<commit_message>
Changes made to files to make them suitable for linux
</commit_message>
<xml_diff>
--- a/Exp Data.xlsx
+++ b/Exp Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="25">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -80,6 +80,21 @@
   </si>
   <si>
     <t xml:space="preserve">50-70%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-50%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40-80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60-95%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90-100%</t>
   </si>
 </sst>
 </file>
@@ -196,15 +211,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10"/>
   </cols>
@@ -599,15 +614,142 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.492</v>
+        <v>0.502</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.6</v>
+        <v>0.61</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.002</v>
-      </c>
-    </row>
+        <v>0.012</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>0.502</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0.502</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>0.502</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>